<commit_message>
production shares with biomass shares
</commit_message>
<xml_diff>
--- a/Plotting/production_shares_ammonia_Scope1-2.xlsx
+++ b/Plotting/production_shares_ammonia_Scope1-2.xlsx
@@ -453,7 +453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -504,13 +504,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>118399.9999999854</v>
+        <v>-3.912214467726298e-08</v>
       </c>
       <c r="C4" t="n">
-        <v>118365.5705865929</v>
+        <v>2664.798010691252</v>
       </c>
       <c r="D4" t="n">
-        <v>117630.122935619</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -520,13 +520,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1065599.999999881</v>
+        <v>35238095.23809128</v>
       </c>
       <c r="C5" t="n">
-        <v>1059194.966100254</v>
+        <v>4630783.093411878</v>
       </c>
       <c r="D5" t="n">
-        <v>1058671.106420491</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -539,7 +539,7 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>-6.409543859914304e-08</v>
+        <v>-2.522017896953197e-07</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
@@ -555,7 +555,7 @@
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>1.346618889584875e-10</v>
+        <v>2.404676588544419e-09</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
@@ -639,6 +639,54 @@
       </c>
       <c r="D12" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>Electrification + Bio-based feedstock</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>-8.923596138608058e-07</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>Conventional + Bio-based feedstock</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>9428.791630345906</v>
+      </c>
+      <c r="D14" t="n">
+        <v>2.114406099842145e-07</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>Conventional + Bio-based feedstock with CC</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>16384990.04349792</v>
+      </c>
+      <c r="D15" t="n">
+        <v>28007172.12752622</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final N-policy linking plots pt 2
</commit_message>
<xml_diff>
--- a/Plotting/production_shares_ammonia_Scope1-2.xlsx
+++ b/Plotting/production_shares_ammonia_Scope1-2.xlsx
@@ -453,7 +453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,6 +488,13 @@
       </c>
       <c r="I1" s="1" t="n"/>
       <c r="J1" s="1" t="n"/>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Iteration_3</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="n"/>
+      <c r="M1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -540,6 +547,21 @@
           <t>2050</t>
         </is>
       </c>
+      <c r="K2" s="1" t="inlineStr">
+        <is>
+          <t>2030</t>
+        </is>
+      </c>
+      <c r="L2" s="1" t="inlineStr">
+        <is>
+          <t>2040</t>
+        </is>
+      </c>
+      <c r="M2" s="1" t="inlineStr">
+        <is>
+          <t>2050</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -557,7 +579,7 @@
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>1183999.999999789</v>
+        <v>1184000.000000019</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
@@ -566,12 +588,21 @@
         <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>1184000.000000012</v>
+        <v>1183999.999999995</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
       </c>
       <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>1184000.00000003</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -608,6 +639,15 @@
       <c r="J5" t="n">
         <v>0</v>
       </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -625,21 +665,30 @@
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>6.977175300198235e-07</v>
+        <v>1.80409352167688e-08</v>
       </c>
       <c r="F6" t="n">
-        <v>1181738.26257592</v>
+        <v>1181739.221044932</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>8.747791622340428e-07</v>
+        <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>1181738.895756663</v>
+        <v>1181734.682806534</v>
       </c>
       <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>1181739.385345381</v>
+      </c>
+      <c r="M6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -659,22 +708,31 @@
         <v>1180474.661760693</v>
       </c>
       <c r="E7" t="n">
-        <v>2.113276659554965e-08</v>
+        <v>1.979831757394561e-10</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>1183903.89879729</v>
+        <v>1183984.965423797</v>
       </c>
       <c r="H7" t="n">
-        <v>-2.758638878031571e-08</v>
+        <v>0</v>
       </c>
       <c r="I7" t="n">
         <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>1183911.436787312</v>
+        <v>1183896.153265644</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>1183897.260867802</v>
       </c>
     </row>
     <row r="8">
@@ -710,6 +768,15 @@
       <c r="J8" t="n">
         <v>0</v>
       </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -744,6 +811,15 @@
       <c r="J9" t="n">
         <v>0</v>
       </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -778,6 +854,15 @@
       <c r="J10" t="n">
         <v>0</v>
       </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -812,6 +897,15 @@
       <c r="J11" t="n">
         <v>0</v>
       </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -846,6 +940,15 @@
       <c r="J12" t="n">
         <v>0</v>
       </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -880,6 +983,15 @@
       <c r="J13" t="n">
         <v>0</v>
       </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -914,6 +1026,15 @@
       <c r="J14" t="n">
         <v>0</v>
       </c>
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -948,12 +1069,22 @@
       <c r="J15" t="n">
         <v>0</v>
       </c>
+      <c r="K15" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
+    <mergeCell ref="K1:M1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>